<commit_message>
Add part of PAM funcs (#27)
* Start PAM

* Add part of PAM funcs
</commit_message>
<xml_diff>
--- a/Documentation/Описание битовых масок СЭС v0.0.xlsx
+++ b/Documentation/Описание битовых масок СЭС v0.0.xlsx
@@ -516,39 +516,6 @@
   </cellStyleXfs>
   <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -592,15 +559,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -627,6 +585,48 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -933,7 +933,7 @@
   <dimension ref="B5:U14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,395 +959,395 @@
   <sheetData>
     <row r="5" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="6"/>
-      <c r="U6" s="7"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
+      <c r="O6" s="37"/>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="37"/>
+      <c r="R6" s="37"/>
+      <c r="S6" s="37"/>
+      <c r="T6" s="37"/>
+      <c r="U6" s="38"/>
     </row>
     <row r="7" spans="2:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="8"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="12">
+      <c r="B7" s="29"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="1">
         <v>15</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="2">
         <v>14</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="2">
         <v>13</v>
       </c>
-      <c r="I7" s="14">
+      <c r="I7" s="3">
         <v>12</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="1">
         <v>11</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K7" s="2">
         <v>10</v>
       </c>
-      <c r="L7" s="13">
+      <c r="L7" s="2">
         <v>9</v>
       </c>
-      <c r="M7" s="15">
+      <c r="M7" s="4">
         <v>8</v>
       </c>
-      <c r="N7" s="12">
+      <c r="N7" s="1">
         <v>7</v>
       </c>
-      <c r="O7" s="13">
+      <c r="O7" s="2">
         <v>6</v>
       </c>
-      <c r="P7" s="13">
+      <c r="P7" s="2">
         <v>5</v>
       </c>
-      <c r="Q7" s="14">
+      <c r="Q7" s="3">
         <v>4</v>
       </c>
-      <c r="R7" s="16">
+      <c r="R7" s="5">
         <v>3</v>
       </c>
-      <c r="S7" s="13">
+      <c r="S7" s="2">
         <v>2</v>
       </c>
-      <c r="T7" s="13">
+      <c r="T7" s="2">
         <v>1</v>
       </c>
-      <c r="U7" s="14">
+      <c r="U7" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:21" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="1">
         <v>16</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="2">
         <v>91</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="1">
         <v>0</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="2">
         <v>0</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="2">
         <v>0</v>
       </c>
-      <c r="I8" s="14">
+      <c r="I8" s="3">
         <v>0</v>
       </c>
-      <c r="J8" s="19" t="s">
+      <c r="J8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="K8" s="20" t="s">
+      <c r="K8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="L8" s="20" t="s">
+      <c r="L8" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="M8" s="21" t="s">
+      <c r="M8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="N8" s="22" t="s">
+      <c r="N8" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="O8" s="23" t="s">
+      <c r="O8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="P8" s="23" t="s">
+      <c r="P8" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="Q8" s="24" t="s">
+      <c r="Q8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="R8" s="19" t="s">
+      <c r="R8" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="S8" s="20" t="s">
+      <c r="S8" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="T8" s="20" t="s">
+      <c r="T8" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="U8" s="25" t="s">
+      <c r="U8" s="14" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="26"/>
-      <c r="O9" s="26"/>
-      <c r="P9" s="26"/>
-      <c r="Q9" s="26"/>
-      <c r="R9" s="26"/>
-      <c r="S9" s="26"/>
-      <c r="T9" s="26"/>
-      <c r="U9" s="26"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15"/>
     </row>
     <row r="10" spans="2:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="27" t="s">
+      <c r="F10" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="28"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="26"/>
-      <c r="P10" s="26"/>
-      <c r="Q10" s="26"/>
-      <c r="R10" s="26"/>
-      <c r="S10" s="26"/>
-      <c r="T10" s="26"/>
-      <c r="U10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="15"/>
+      <c r="T10" s="15"/>
+      <c r="U10" s="15"/>
     </row>
     <row r="11" spans="2:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="30">
+      <c r="B11" s="29"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="16">
         <v>7</v>
       </c>
-      <c r="G11" s="31">
+      <c r="G11" s="17">
         <v>6</v>
       </c>
-      <c r="H11" s="31">
+      <c r="H11" s="17">
         <v>5</v>
       </c>
-      <c r="I11" s="32">
+      <c r="I11" s="18">
         <v>4</v>
       </c>
-      <c r="J11" s="33">
+      <c r="J11" s="19">
         <v>3</v>
       </c>
-      <c r="K11" s="31">
+      <c r="K11" s="17">
         <v>2</v>
       </c>
-      <c r="L11" s="31">
+      <c r="L11" s="17">
         <v>1</v>
       </c>
-      <c r="M11" s="32">
+      <c r="M11" s="18">
         <v>0</v>
       </c>
-      <c r="N11" s="26"/>
-      <c r="O11" s="26"/>
-      <c r="P11" s="26"/>
-      <c r="Q11" s="26"/>
-      <c r="R11" s="26"/>
-      <c r="S11" s="26"/>
-      <c r="T11" s="26"/>
-      <c r="U11" s="26"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
     </row>
     <row r="12" spans="2:21" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="1">
         <v>8</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="2">
         <v>88</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="22" t="s">
+      <c r="F12" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="23" t="s">
+      <c r="G12" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="H12" s="23" t="s">
+      <c r="H12" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="I12" s="24" t="s">
+      <c r="I12" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="J12" s="34" t="s">
+      <c r="J12" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K12" s="23" t="s">
+      <c r="K12" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="L12" s="23" t="s">
+      <c r="L12" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="M12" s="24" t="s">
+      <c r="M12" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="N12" s="26"/>
-      <c r="O12" s="26"/>
-      <c r="P12" s="26"/>
-      <c r="Q12" s="26"/>
-      <c r="R12" s="26"/>
-      <c r="S12" s="26"/>
-      <c r="T12" s="26"/>
-      <c r="U12" s="26"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="15"/>
+      <c r="T12" s="15"/>
+      <c r="U12" s="15"/>
     </row>
     <row r="13" spans="2:21" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="36">
+      <c r="C13" s="22">
         <v>8</v>
       </c>
-      <c r="D13" s="37">
-        <v>88</v>
-      </c>
-      <c r="E13" s="38" t="s">
+      <c r="D13" s="23">
+        <v>89</v>
+      </c>
+      <c r="E13" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="22" t="s">
+      <c r="F13" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="23" t="s">
+      <c r="G13" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="H13" s="23" t="s">
+      <c r="H13" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="I13" s="24" t="s">
+      <c r="I13" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="J13" s="34" t="s">
+      <c r="J13" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K13" s="23" t="s">
+      <c r="K13" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="L13" s="23" t="s">
+      <c r="L13" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="M13" s="24" t="s">
+      <c r="M13" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="N13" s="26"/>
-      <c r="O13" s="26"/>
-      <c r="P13" s="26"/>
-      <c r="Q13" s="26"/>
-      <c r="R13" s="26"/>
-      <c r="S13" s="26"/>
-      <c r="T13" s="26"/>
-      <c r="U13" s="26"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="15"/>
+      <c r="U13" s="15"/>
     </row>
     <row r="14" spans="2:21" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="36">
+      <c r="C14" s="22">
         <v>8</v>
       </c>
-      <c r="D14" s="37">
-        <v>88</v>
-      </c>
-      <c r="E14" s="38" t="s">
+      <c r="D14" s="23">
+        <v>90</v>
+      </c>
+      <c r="E14" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="22" t="s">
+      <c r="F14" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="23" t="s">
+      <c r="G14" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="H14" s="23" t="s">
+      <c r="H14" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="I14" s="24" t="s">
+      <c r="I14" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="J14" s="34" t="s">
+      <c r="J14" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K14" s="23" t="s">
+      <c r="K14" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="L14" s="23" t="s">
+      <c r="L14" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="M14" s="24" t="s">
+      <c r="M14" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="N14" s="26"/>
-      <c r="O14" s="26"/>
-      <c r="P14" s="26"/>
-      <c r="Q14" s="26"/>
-      <c r="R14" s="26"/>
-      <c r="S14" s="26"/>
-      <c r="T14" s="26"/>
-      <c r="U14" s="26"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="15"/>
+      <c r="S14" s="15"/>
+      <c r="T14" s="15"/>
+      <c r="U14" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="F6:U6"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
     <mergeCell ref="F10:M10"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F6:U6"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>